<commit_message>
Updated the design - Stable design
</commit_message>
<xml_diff>
--- a/Components/Qwiic_Adaptive_Switch_BOM.xlsx
+++ b/Components/Qwiic_Adaptive_Switch_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milad\Development\Personal\Qwiic-Adaptive-Switch\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3FBD5A-2783-4227-B6F6-D1062E36BB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F187F832-9D57-43CF-8D3C-8765A6A34A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5293" yWindow="2927" windowWidth="19200" windowHeight="11273" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Qwiic_Adaptive_Switch_BOM" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Index</t>
   </si>
@@ -78,9 +78,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>J2,J3</t>
-  </si>
-  <si>
     <t>PRT-14417-ND</t>
   </si>
   <si>
@@ -105,30 +102,6 @@
     <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-072K2L/727016</t>
   </si>
   <si>
-    <t>311-10KDTR-ND</t>
-  </si>
-  <si>
-    <t>RT0603DRD0710KL</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 0.5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/yageo/RT0603DRD0710KL/1035416</t>
-  </si>
-  <si>
-    <t>YAG1237TR-ND</t>
-  </si>
-  <si>
-    <t>RT0603BRD071KL</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 0.1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/yageo/RT0603BRD071KL/1072344</t>
-  </si>
-  <si>
     <t>587-1245-2-ND</t>
   </si>
   <si>
@@ -192,17 +165,61 @@
     <t>2.2K</t>
   </si>
   <si>
-    <t xml:space="preserve">	
-QWIIC JST</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
     <t>R3</t>
   </si>
   <si>
-    <t>R1,R2,R5,R6,R7,R8,R9</t>
+    <t>R1,R2,R7,R8,R9</t>
+  </si>
+  <si>
+    <t>R5,R6</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>311-4.7KGRTR-ND</t>
+  </si>
+  <si>
+    <t>RC0603JR-074K7L</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603JR-074K7L/726785</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603JR-0710KL/726700</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-10KGRTR-ND </t>
+  </si>
+  <si>
+    <t>RC0603JR-0710KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/yageo/RC0603FR-071KL/726843</t>
+  </si>
+  <si>
+    <t>311-1.00KHRTR-ND</t>
+  </si>
+  <si>
+    <t>RC0603FR-071KL</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>QWIIC JST</t>
+  </si>
+  <si>
+    <t>J1,J3</t>
   </si>
 </sst>
 </file>
@@ -1060,15 +1077,15 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1096,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1100,7 +1117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1128,11 +1145,11 @@
       <c r="I2">
         <v>1.97</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1143,16 +1160,16 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H3">
         <v>1.82</v>
@@ -1160,11 +1177,11 @@
       <c r="I3">
         <v>1.82</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>44</v>
+      <c r="J3" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1172,19 +1189,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
       </c>
       <c r="H4">
         <v>0.69</v>
@@ -1192,31 +1209,31 @@
       <c r="I4">
         <v>0.69</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
+      <c r="J4" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
       </c>
       <c r="H5">
         <v>0.15</v>
@@ -1224,11 +1241,11 @@
       <c r="I5">
         <v>0.15</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>23</v>
+      <c r="J5" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1236,31 +1253,31 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
         <v>55</v>
       </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H6">
-        <v>0.25</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I6">
-        <v>0.25</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1268,63 +1285,63 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H7">
-        <v>0.47</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I7">
-        <v>0.47</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
         <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="H8">
-        <v>0.14000000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="I8">
         <v>0.14000000000000001</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1332,49 +1349,78 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9">
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10">
         <v>0.33</v>
       </c>
-      <c r="I9">
+      <c r="I10">
         <v>0.33</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>39</v>
+      <c r="J10" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="H13" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="I13">
-        <f>H2*B2+H3*B3+H4*B4+H5*B5+H6*B6+H7*B7+H8*B8+H9*B9</f>
-        <v>9.3800000000000008</v>
+        <f>H2*B2+H3*B3+H4*B4+H5*B5+H6*B6+H7*B7+H8*B8+H9*B9+H10*B10</f>
+        <v>9.14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J8" r:id="rId1" xr:uid="{7CFB89AE-3D4D-4CA9-B93C-DCC08D3DA9CE}"/>
-    <hyperlink ref="J9" r:id="rId2" xr:uid="{302D5C69-202C-4864-974C-E201C538E929}"/>
-    <hyperlink ref="J7" r:id="rId3" xr:uid="{65D4B927-EC5B-49D1-B880-42371423F319}"/>
-    <hyperlink ref="J6" r:id="rId4" xr:uid="{DAF42746-61D3-45DF-8D5F-5877A0BDE783}"/>
-    <hyperlink ref="J5" r:id="rId5" xr:uid="{EC465C77-9FC5-474C-A61A-5C7BBFC37E55}"/>
-    <hyperlink ref="J3" r:id="rId6" xr:uid="{AE3C2BE3-D8F3-46EC-8BC6-61EF2C802E50}"/>
-    <hyperlink ref="J2" r:id="rId7" xr:uid="{FA1A89EA-09EA-4668-9F95-F10032EFB685}"/>
-    <hyperlink ref="J4" r:id="rId8" xr:uid="{FA24F7A0-85F2-4300-90CB-2A9426B2C7C6}"/>
+    <hyperlink ref="J8" r:id="rId1" xr:uid="{57F48D8A-3087-47C8-A385-FEC943BA2F89}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{303FD325-93A2-4122-A17E-C111FE863494}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{45ABB9EA-EB9F-4A28-9ABF-7C64A3A6F5DB}"/>
+    <hyperlink ref="J9" r:id="rId4" xr:uid="{9B4361CF-880F-4767-81AA-95457881CD70}"/>
+    <hyperlink ref="J10" r:id="rId5" xr:uid="{3E4978E0-C4E0-49A4-8EB1-E99414799B0D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>